<commit_message>
created api to find job
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="1088">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="1114">
   <si>
     <t>register_complete</t>
   </si>
@@ -3304,6 +3304,84 @@
   </si>
   <si>
     <t>I'm passionate about management and i'm able to leadership </t>
+  </si>
+  <si>
+    <t>Kajal</t>
+  </si>
+  <si>
+    <t>Sharma </t>
+  </si>
+  <si>
+    <t>kvskajalsharma10@gmail.com</t>
+  </si>
+  <si>
+    <t>8010844492</t>
+  </si>
+  <si>
+    <t>Kajal@123</t>
+  </si>
+  <si>
+    <t>WiFUGhCVpmNtX1kBruZ2th6l4</t>
+  </si>
+  <si>
+    <t>https://rekonnectfileupload.s3.ap-south-1.amazonaws.com/RekonnectKajal%20Sharma%20resume.pdf</t>
+  </si>
+  <si>
+    <t>Business development,Bach office work, I can do all types work from home </t>
+  </si>
+  <si>
+    <t>Sarita</t>
+  </si>
+  <si>
+    <t>sarita7july@gmail.com</t>
+  </si>
+  <si>
+    <t>9518168616</t>
+  </si>
+  <si>
+    <t>snutrition2021</t>
+  </si>
+  <si>
+    <t>dzcqtJSSIUSCDZdxRwcMldeu6</t>
+  </si>
+  <si>
+    <t>https://rekonnectfileupload.s3.ap-south-1.amazonaws.com/RekonnectSarita%20Biodata.pdf</t>
+  </si>
+  <si>
+    <t>As a web developer</t>
+  </si>
+  <si>
+    <t>Gaurav</t>
+  </si>
+  <si>
+    <t>kgaurav.developer@gmail.com</t>
+  </si>
+  <si>
+    <t>WlYeGWdam259oMdAdgK7tsw6u</t>
+  </si>
+  <si>
+    <t>https://rekonnectfileupload.s3.ap-south-1.amazonaws.com/RekonnectGaurav%27s%20Resume.pdf</t>
+  </si>
+  <si>
+    <t>I WANT TO BECOME A SUCCESSFUL ANDROID APP DEVELOPER</t>
+  </si>
+  <si>
+    <t>Preksha</t>
+  </si>
+  <si>
+    <t>Sethia</t>
+  </si>
+  <si>
+    <t>prekshasethia4@gmail.com</t>
+  </si>
+  <si>
+    <t>nKE4wnfkD9TTxRplggQ5TF6mO</t>
+  </si>
+  <si>
+    <t>https://rekonnectfileupload.s3.ap-south-1.amazonaws.com/Rekonnect1624557057862Resume_Preksha.docx</t>
+  </si>
+  <si>
+    <t>I m passionate about learning new things</t>
   </si>
 </sst>
 </file>
@@ -3343,7 +3421,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE159"/>
+  <dimension ref="A1:AE163"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -18232,6 +18310,374 @@
         <v>63</v>
       </c>
     </row>
+    <row r="160" spans="1:31">
+      <c r="A160" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B160" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C160" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D160" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E160" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F160" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="G160" s="0" t="s">
+        <v>1088</v>
+      </c>
+      <c r="H160" s="0" t="s">
+        <v>1089</v>
+      </c>
+      <c r="I160" s="0" t="s">
+        <v>1090</v>
+      </c>
+      <c r="J160" s="0" t="s">
+        <v>1091</v>
+      </c>
+      <c r="K160" s="0" t="s">
+        <v>1092</v>
+      </c>
+      <c r="L160" s="0" t="s">
+        <v>1093</v>
+      </c>
+      <c r="M160" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="N160" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="O160" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="P160" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q160" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="R160" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="S160" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T160" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="U160" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="V160" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="W160" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="X160" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y160" s="0" t="s">
+        <v>1094</v>
+      </c>
+      <c r="Z160" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA160" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB160" s="0" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AC160" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD160" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE160" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="161" spans="1:31">
+      <c r="A161" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B161" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C161" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D161" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E161" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F161" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="G161" s="0" t="s">
+        <v>1096</v>
+      </c>
+      <c r="H161" s="0" t="s">
+        <v>1096</v>
+      </c>
+      <c r="I161" s="0" t="s">
+        <v>1097</v>
+      </c>
+      <c r="J161" s="0" t="s">
+        <v>1098</v>
+      </c>
+      <c r="K161" s="0" t="s">
+        <v>1099</v>
+      </c>
+      <c r="L161" s="0" t="s">
+        <v>1100</v>
+      </c>
+      <c r="M161" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="N161" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="O161" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="P161" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q161" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="R161" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="S161" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T161" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="U161" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="V161" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="W161" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="X161" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y161" s="0" t="s">
+        <v>1101</v>
+      </c>
+      <c r="Z161" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA161" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB161" s="0" t="s">
+        <v>1102</v>
+      </c>
+      <c r="AC161" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD161" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE161" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="162" spans="1:29">
+      <c r="A162" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B162" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C162" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D162" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E162" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F162" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="G162" s="0" t="s">
+        <v>511</v>
+      </c>
+      <c r="H162" s="0" t="s">
+        <v>1103</v>
+      </c>
+      <c r="I162" s="0" t="s">
+        <v>1104</v>
+      </c>
+      <c r="J162" s="0" t="s">
+        <v>1105</v>
+      </c>
+      <c r="K162" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="L162" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M162" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="N162" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="O162" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="P162" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q162" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="R162" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="S162" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T162" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="U162" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="V162" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="W162" s="0" t="s">
+        <v>1106</v>
+      </c>
+      <c r="X162" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y162" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z162" s="0" t="s">
+        <v>1107</v>
+      </c>
+      <c r="AA162" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB162" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC162" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="163" spans="1:29">
+      <c r="A163" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B163" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C163" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D163" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E163" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F163" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="G163" s="0" t="s">
+        <v>1108</v>
+      </c>
+      <c r="H163" s="0" t="s">
+        <v>1109</v>
+      </c>
+      <c r="I163" s="0" t="s">
+        <v>1110</v>
+      </c>
+      <c r="J163" s="0" t="s">
+        <v>1111</v>
+      </c>
+      <c r="K163" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="L163" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M163" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="N163" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="O163" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="P163" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q163" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="R163" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="S163" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T163" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="U163" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="V163" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="W163" s="0" t="s">
+        <v>1112</v>
+      </c>
+      <c r="X163" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y163" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z163" s="0" t="s">
+        <v>1113</v>
+      </c>
+      <c r="AA163" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB163" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC163" s="0" t="s">
+        <v>103</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added hash funtionalinty tesst
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1324" uniqueCount="1324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1435" uniqueCount="1435">
   <si>
     <t>register_complete</t>
   </si>
@@ -4012,6 +4012,339 @@
   </si>
   <si>
     <t>713201</t>
+  </si>
+  <si>
+    <t>1260</t>
+  </si>
+  <si>
+    <t>pavan</t>
+  </si>
+  <si>
+    <t>pavanpk3563@gmail.com</t>
+  </si>
+  <si>
+    <t>mjTnZLlvtBWfOdAc3wWJAqy3G</t>
+  </si>
+  <si>
+    <t>https://rekonnectfileupload.s3.ap-south-1.amazonaws.com/Rekonnectmine.jpeg</t>
+  </si>
+  <si>
+    <t>https://rekonnectfileupload.s3.ap-south-1.amazonaws.com/Rekonnectresume.pdf</t>
+  </si>
+  <si>
+    <t>..</t>
+  </si>
+  <si>
+    <t>535161</t>
+  </si>
+  <si>
+    <t>kashyapi</t>
+  </si>
+  <si>
+    <t>Gautam</t>
+  </si>
+  <si>
+    <t>kashyapigautam02@gmail.com</t>
+  </si>
+  <si>
+    <t>9040455246</t>
+  </si>
+  <si>
+    <t>Femina@02</t>
+  </si>
+  <si>
+    <t>t50Bjjqr2d6bhLEIQJf7a8Ab5</t>
+  </si>
+  <si>
+    <t>https://rekonnectfileupload.s3.ap-south-1.amazonaws.com/RekonnectKashyapi_Gautam_Resume_04-04-2022-18-26-51.pdf</t>
+  </si>
+  <si>
+    <t>Reading books, travelling, dancing</t>
+  </si>
+  <si>
+    <t>411016</t>
+  </si>
+  <si>
+    <t>Harshit</t>
+  </si>
+  <si>
+    <t>harshitsingh8456@gmail.com</t>
+  </si>
+  <si>
+    <t>7pdLsgEj3FKH0xxPMbKcitc2Z</t>
+  </si>
+  <si>
+    <t>https://rekonnectfileupload.s3.ap-south-1.amazonaws.com/RekonnectHarshit%20photo.jpeg</t>
+  </si>
+  <si>
+    <t>https://rekonnectfileupload.s3.ap-south-1.amazonaws.com/RekonnectHarshit%27s%20Resume%20%289%29.pdf</t>
+  </si>
+  <si>
+    <t>To being a best developer</t>
+  </si>
+  <si>
+    <t>400608</t>
+  </si>
+  <si>
+    <t>Sujit Kumar</t>
+  </si>
+  <si>
+    <t>Sahoo</t>
+  </si>
+  <si>
+    <t>sujit7008680226@gmail.com</t>
+  </si>
+  <si>
+    <t>7008680226</t>
+  </si>
+  <si>
+    <t>Sujit@123</t>
+  </si>
+  <si>
+    <t>oMCo9vhB27JpK3K0pqv4LvTdV</t>
+  </si>
+  <si>
+    <t>https://rekonnectfileupload.s3.ap-south-1.amazonaws.com/RekonnectIMG_20211229_220453_1%20-%20Copy.jpg</t>
+  </si>
+  <si>
+    <t>https://rekonnectfileupload.s3.ap-south-1.amazonaws.com/RekonnectSUJIT%20KUMAR%20SAHOO-converted.pdf</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>756101</t>
+  </si>
+  <si>
+    <t>Minal</t>
+  </si>
+  <si>
+    <t>Saini</t>
+  </si>
+  <si>
+    <t>minalsaini2525@gmail.com</t>
+  </si>
+  <si>
+    <t>9205751520</t>
+  </si>
+  <si>
+    <t>Gopal@2510</t>
+  </si>
+  <si>
+    <t>F8eJxk3VBzKwiYgxZ4qIap7P4</t>
+  </si>
+  <si>
+    <t>Need a good master in this skill</t>
+  </si>
+  <si>
+    <t>110088</t>
+  </si>
+  <si>
+    <t>Nisha</t>
+  </si>
+  <si>
+    <t>Gadling</t>
+  </si>
+  <si>
+    <t>gadlingnisha.13@gmail.com</t>
+  </si>
+  <si>
+    <t>7225903868</t>
+  </si>
+  <si>
+    <t>Nisha@99</t>
+  </si>
+  <si>
+    <t>vxN0AuTqkUfVsMOLRz7UE9glj</t>
+  </si>
+  <si>
+    <t>https://rekonnectfileupload.s3.ap-south-1.amazonaws.com/RekonnectNisha-Resume.docx</t>
+  </si>
+  <si>
+    <t>I am passionate about my work I really want to explore my knowledge and skills into the organisation</t>
+  </si>
+  <si>
+    <t>444905</t>
+  </si>
+  <si>
+    <t>Komal</t>
+  </si>
+  <si>
+    <t>Tehare</t>
+  </si>
+  <si>
+    <t>komalkpt1997@gmail.com</t>
+  </si>
+  <si>
+    <t>8975088658</t>
+  </si>
+  <si>
+    <t>KPTspt1997@#$</t>
+  </si>
+  <si>
+    <t>0YFpiT7I7PLCKmbQye1k3S5Ni</t>
+  </si>
+  <si>
+    <t>Softwa</t>
+  </si>
+  <si>
+    <t>411014</t>
+  </si>
+  <si>
+    <t>kunal</t>
+  </si>
+  <si>
+    <t>krishna</t>
+  </si>
+  <si>
+    <t>kunalkrishnahr@gmail.com</t>
+  </si>
+  <si>
+    <t>7651815919</t>
+  </si>
+  <si>
+    <t>jaishreeram</t>
+  </si>
+  <si>
+    <t>F0N8IHfRuQhQu1YNL3VL2cgiL</t>
+  </si>
+  <si>
+    <t>https://rekonnectfileupload.s3.ap-south-1.amazonaws.com/Rekonnectkunal%20krishna%20updated%20resume%20latest-1.docx</t>
+  </si>
+  <si>
+    <t>hr</t>
+  </si>
+  <si>
+    <t>226201</t>
+  </si>
+  <si>
+    <t>Niketa </t>
+  </si>
+  <si>
+    <t>singh.niketa99@gmail.com</t>
+  </si>
+  <si>
+    <t>9971876306</t>
+  </si>
+  <si>
+    <t>spicy@sugar1234</t>
+  </si>
+  <si>
+    <t>Q56PMgi3DsRKjWznq0Hvxxdkf</t>
+  </si>
+  <si>
+    <t>I love being active part of any activity</t>
+  </si>
+  <si>
+    <t>201005</t>
+  </si>
+  <si>
+    <t>swati</t>
+  </si>
+  <si>
+    <t>inventiway</t>
+  </si>
+  <si>
+    <t>sinventiway@gmail.com</t>
+  </si>
+  <si>
+    <t>YlnQtv9AoRGdkIkxKfiHOo5l0</t>
+  </si>
+  <si>
+    <t>tax</t>
+  </si>
+  <si>
+    <t>71111110</t>
+  </si>
+  <si>
+    <t>pihu</t>
+  </si>
+  <si>
+    <t>saxena</t>
+  </si>
+  <si>
+    <t>pihusaxena17@gmail.com</t>
+  </si>
+  <si>
+    <t>w4sSZIGqjs1bhABwcCTl5iZZ6</t>
+  </si>
+  <si>
+    <t>https://rekonnectfileupload.s3.ap-south-1.amazonaws.com/RekonnectPOOJA%20SAXENA%20update%20CV%208%20may%20pdf.pdf</t>
+  </si>
+  <si>
+    <t>Teaching is my passion but engineering is my professional life , so I eagerly want to grow in software testing industry </t>
+  </si>
+  <si>
+    <t>110055</t>
+  </si>
+  <si>
+    <t>PREETI SAI </t>
+  </si>
+  <si>
+    <t>THANDAVAN </t>
+  </si>
+  <si>
+    <t>preetisai.thandavan2020@vitstudent.ac.in</t>
+  </si>
+  <si>
+    <t>9176056214</t>
+  </si>
+  <si>
+    <t>p1r2e3e4t5i6</t>
+  </si>
+  <si>
+    <t>oUajbrgGupWYfxVC0QfGyaY9z</t>
+  </si>
+  <si>
+    <t>I would want to make wonders in the field of IT </t>
+  </si>
+  <si>
+    <t>603103</t>
+  </si>
+  <si>
+    <t>Ashish</t>
+  </si>
+  <si>
+    <t>ak2917065@gmail.com</t>
+  </si>
+  <si>
+    <t>9653662159</t>
+  </si>
+  <si>
+    <t>Ashish@1</t>
+  </si>
+  <si>
+    <t>JVW1bxDkk4EdFp9CNm9dvvlA9</t>
+  </si>
+  <si>
+    <t>https://rekonnectfileupload.s3.ap-south-1.amazonaws.com/RekonnectAshish_Kumar_Resume%28flutter%29.pdf</t>
+  </si>
+  <si>
+    <t>I have passion of developing mobile application and programming. I love to build application for real world problems. </t>
+  </si>
+  <si>
+    <t>Ruma</t>
+  </si>
+  <si>
+    <t>Yadav</t>
+  </si>
+  <si>
+    <t>yruma2007@gmail.com</t>
+  </si>
+  <si>
+    <t>9330380800</t>
+  </si>
+  <si>
+    <t>Mky@123456</t>
+  </si>
+  <si>
+    <t>TPXqI2RdeM6ZriBFynh8qyfrw</t>
+  </si>
+  <si>
+    <t>Nothing much wanted to learn everyday</t>
+  </si>
+  <si>
+    <t>711101</t>
   </si>
 </sst>
 </file>
@@ -4051,7 +4384,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ167"/>
+  <dimension ref="A1:AJ181"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -22187,6 +22520,1528 @@
         <v>1323</v>
       </c>
     </row>
+    <row r="168" spans="1:34">
+      <c r="A168" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B168" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C168" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D168" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E168" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F168" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G168" s="0" t="s">
+        <v>1324</v>
+      </c>
+      <c r="H168" s="0" t="s">
+        <v>1325</v>
+      </c>
+      <c r="I168" s="0" t="s">
+        <v>1326</v>
+      </c>
+      <c r="J168" s="0" t="s">
+        <v>1327</v>
+      </c>
+      <c r="K168" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="L168" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="M168" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="N168" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="O168" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="P168" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q168" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="R168" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="S168" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="T168" s="0" t="s">
+        <v>1328</v>
+      </c>
+      <c r="U168" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="V168" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="W168" s="0" t="s">
+        <v>1329</v>
+      </c>
+      <c r="X168" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y168" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z168" s="0" t="s">
+        <v>1330</v>
+      </c>
+      <c r="AA168" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB168" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC168" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD168" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE168" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF168" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG168" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="AH168" s="0" t="s">
+        <v>1331</v>
+      </c>
+    </row>
+    <row r="169" spans="1:36">
+      <c r="A169" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B169" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C169" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D169" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E169" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F169" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G169" s="0" t="s">
+        <v>1332</v>
+      </c>
+      <c r="H169" s="0" t="s">
+        <v>1333</v>
+      </c>
+      <c r="I169" s="0" t="s">
+        <v>1334</v>
+      </c>
+      <c r="J169" s="0" t="s">
+        <v>1335</v>
+      </c>
+      <c r="K169" s="0" t="s">
+        <v>1336</v>
+      </c>
+      <c r="L169" s="0" t="s">
+        <v>1337</v>
+      </c>
+      <c r="M169" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="N169" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="O169" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="P169" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q169" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="R169" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="S169" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="T169" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="U169" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="V169" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="W169" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="X169" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y169" s="0" t="s">
+        <v>1338</v>
+      </c>
+      <c r="Z169" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA169" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB169" s="0" t="s">
+        <v>1339</v>
+      </c>
+      <c r="AC169" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD169" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE169" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF169" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG169" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH169" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="AI169" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="AJ169" s="0" t="s">
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="170" spans="1:34">
+      <c r="A170" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B170" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C170" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D170" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E170" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F170" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G170" s="0" t="s">
+        <v>1341</v>
+      </c>
+      <c r="H170" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="I170" s="0" t="s">
+        <v>1342</v>
+      </c>
+      <c r="J170" s="0" t="s">
+        <v>1343</v>
+      </c>
+      <c r="K170" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="L170" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="M170" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="N170" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="O170" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="P170" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q170" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="R170" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="S170" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="T170" s="0" t="s">
+        <v>1344</v>
+      </c>
+      <c r="U170" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="V170" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="W170" s="0" t="s">
+        <v>1345</v>
+      </c>
+      <c r="X170" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y170" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z170" s="0" t="s">
+        <v>1346</v>
+      </c>
+      <c r="AA170" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB170" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC170" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD170" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE170" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF170" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="AG170" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="AH170" s="0" t="s">
+        <v>1347</v>
+      </c>
+    </row>
+    <row r="171" spans="1:36">
+      <c r="A171" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B171" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C171" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D171" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E171" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F171" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G171" s="0" t="s">
+        <v>1348</v>
+      </c>
+      <c r="H171" s="0" t="s">
+        <v>1349</v>
+      </c>
+      <c r="I171" s="0" t="s">
+        <v>1350</v>
+      </c>
+      <c r="J171" s="0" t="s">
+        <v>1351</v>
+      </c>
+      <c r="K171" s="0" t="s">
+        <v>1352</v>
+      </c>
+      <c r="L171" s="0" t="s">
+        <v>1353</v>
+      </c>
+      <c r="M171" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="N171" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="O171" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="P171" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q171" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="R171" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="S171" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="T171" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="U171" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="V171" s="0" t="s">
+        <v>1354</v>
+      </c>
+      <c r="W171" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="X171" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y171" s="0" t="s">
+        <v>1355</v>
+      </c>
+      <c r="Z171" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA171" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB171" s="0" t="s">
+        <v>1356</v>
+      </c>
+      <c r="AC171" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD171" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE171" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="AF171" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG171" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH171" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI171" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="AJ171" s="0" t="s">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="172" spans="1:36">
+      <c r="A172" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B172" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C172" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D172" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E172" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F172" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G172" s="0" t="s">
+        <v>1358</v>
+      </c>
+      <c r="H172" s="0" t="s">
+        <v>1359</v>
+      </c>
+      <c r="I172" s="0" t="s">
+        <v>1360</v>
+      </c>
+      <c r="J172" s="0" t="s">
+        <v>1361</v>
+      </c>
+      <c r="K172" s="0" t="s">
+        <v>1362</v>
+      </c>
+      <c r="L172" s="0" t="s">
+        <v>1363</v>
+      </c>
+      <c r="M172" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="N172" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="O172" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="P172" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q172" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="R172" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="S172" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="T172" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="U172" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="V172" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="W172" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="X172" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y172" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z172" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA172" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB172" s="0" t="s">
+        <v>1364</v>
+      </c>
+      <c r="AC172" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD172" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE172" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF172" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG172" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH172" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI172" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="AJ172" s="0" t="s">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="173" spans="1:36">
+      <c r="A173" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B173" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C173" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D173" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E173" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F173" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G173" s="0" t="s">
+        <v>1366</v>
+      </c>
+      <c r="H173" s="0" t="s">
+        <v>1367</v>
+      </c>
+      <c r="I173" s="0" t="s">
+        <v>1368</v>
+      </c>
+      <c r="J173" s="0" t="s">
+        <v>1369</v>
+      </c>
+      <c r="K173" s="0" t="s">
+        <v>1370</v>
+      </c>
+      <c r="L173" s="0" t="s">
+        <v>1371</v>
+      </c>
+      <c r="M173" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="N173" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="O173" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="P173" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q173" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="R173" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="S173" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="T173" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="U173" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="V173" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="W173" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="X173" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y173" s="0" t="s">
+        <v>1372</v>
+      </c>
+      <c r="Z173" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA173" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB173" s="0" t="s">
+        <v>1373</v>
+      </c>
+      <c r="AC173" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD173" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE173" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF173" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG173" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH173" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI173" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="AJ173" s="0" t="s">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="174" spans="1:36">
+      <c r="A174" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B174" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C174" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D174" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E174" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F174" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G174" s="0" t="s">
+        <v>1375</v>
+      </c>
+      <c r="H174" s="0" t="s">
+        <v>1376</v>
+      </c>
+      <c r="I174" s="0" t="s">
+        <v>1377</v>
+      </c>
+      <c r="J174" s="0" t="s">
+        <v>1378</v>
+      </c>
+      <c r="K174" s="0" t="s">
+        <v>1379</v>
+      </c>
+      <c r="L174" s="0" t="s">
+        <v>1380</v>
+      </c>
+      <c r="M174" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="N174" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="O174" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="P174" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q174" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="R174" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="S174" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="T174" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="U174" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="V174" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="W174" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="X174" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y174" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z174" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA174" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB174" s="0" t="s">
+        <v>1381</v>
+      </c>
+      <c r="AC174" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD174" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE174" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AF174" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG174" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH174" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI174" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="AJ174" s="0" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="175" spans="1:36">
+      <c r="A175" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B175" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C175" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D175" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E175" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F175" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G175" s="0" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H175" s="0" t="s">
+        <v>1384</v>
+      </c>
+      <c r="I175" s="0" t="s">
+        <v>1385</v>
+      </c>
+      <c r="J175" s="0" t="s">
+        <v>1386</v>
+      </c>
+      <c r="K175" s="0" t="s">
+        <v>1387</v>
+      </c>
+      <c r="L175" s="0" t="s">
+        <v>1388</v>
+      </c>
+      <c r="M175" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="N175" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="O175" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="P175" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q175" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="R175" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="S175" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="T175" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="U175" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="V175" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="W175" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="X175" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y175" s="0" t="s">
+        <v>1389</v>
+      </c>
+      <c r="Z175" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA175" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB175" s="0" t="s">
+        <v>1390</v>
+      </c>
+      <c r="AC175" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD175" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE175" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF175" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG175" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH175" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI175" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="AJ175" s="0" t="s">
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="176" spans="1:36">
+      <c r="A176" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B176" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C176" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D176" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E176" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F176" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G176" s="0" t="s">
+        <v>1392</v>
+      </c>
+      <c r="H176" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="I176" s="0" t="s">
+        <v>1393</v>
+      </c>
+      <c r="J176" s="0" t="s">
+        <v>1394</v>
+      </c>
+      <c r="K176" s="0" t="s">
+        <v>1395</v>
+      </c>
+      <c r="L176" s="0" t="s">
+        <v>1396</v>
+      </c>
+      <c r="M176" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="N176" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="O176" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="P176" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q176" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="R176" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="S176" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="T176" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="U176" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="V176" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="W176" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="X176" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y176" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z176" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA176" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB176" s="0" t="s">
+        <v>1397</v>
+      </c>
+      <c r="AC176" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD176" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE176" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF176" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG176" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH176" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="AI176" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="AJ176" s="0" t="s">
+        <v>1398</v>
+      </c>
+    </row>
+    <row r="177" spans="1:36">
+      <c r="A177" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B177" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C177" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D177" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E177" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F177" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G177" s="0" t="s">
+        <v>1399</v>
+      </c>
+      <c r="H177" s="0" t="s">
+        <v>1400</v>
+      </c>
+      <c r="I177" s="0" t="s">
+        <v>1401</v>
+      </c>
+      <c r="J177" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="K177" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="L177" s="0" t="s">
+        <v>1402</v>
+      </c>
+      <c r="M177" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="N177" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="O177" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="P177" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q177" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="R177" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="S177" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="T177" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="U177" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="V177" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="W177" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="X177" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y177" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z177" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA177" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB177" s="0" t="s">
+        <v>1403</v>
+      </c>
+      <c r="AC177" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD177" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE177" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF177" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG177" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH177" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="AI177" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ177" s="0" t="s">
+        <v>1404</v>
+      </c>
+    </row>
+    <row r="178" spans="1:34">
+      <c r="A178" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B178" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C178" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D178" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E178" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F178" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G178" s="0" t="s">
+        <v>1405</v>
+      </c>
+      <c r="H178" s="0" t="s">
+        <v>1406</v>
+      </c>
+      <c r="I178" s="0" t="s">
+        <v>1407</v>
+      </c>
+      <c r="J178" s="0" t="s">
+        <v>1408</v>
+      </c>
+      <c r="K178" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="L178" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="M178" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="N178" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="O178" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="P178" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q178" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="R178" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="S178" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="T178" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="U178" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="V178" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="W178" s="0" t="s">
+        <v>1409</v>
+      </c>
+      <c r="X178" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y178" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z178" s="0" t="s">
+        <v>1410</v>
+      </c>
+      <c r="AA178" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB178" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC178" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD178" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE178" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF178" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG178" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="AH178" s="0" t="s">
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="179" spans="1:36">
+      <c r="A179" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B179" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C179" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D179" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E179" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F179" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G179" s="0" t="s">
+        <v>1412</v>
+      </c>
+      <c r="H179" s="0" t="s">
+        <v>1413</v>
+      </c>
+      <c r="I179" s="0" t="s">
+        <v>1414</v>
+      </c>
+      <c r="J179" s="0" t="s">
+        <v>1415</v>
+      </c>
+      <c r="K179" s="0" t="s">
+        <v>1416</v>
+      </c>
+      <c r="L179" s="0" t="s">
+        <v>1417</v>
+      </c>
+      <c r="M179" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="N179" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="O179" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="P179" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q179" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="R179" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="S179" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="T179" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="U179" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="V179" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="W179" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="X179" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y179" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z179" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA179" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB179" s="0" t="s">
+        <v>1418</v>
+      </c>
+      <c r="AC179" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD179" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE179" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF179" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG179" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH179" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI179" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="AJ179" s="0" t="s">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="180" spans="1:36">
+      <c r="A180" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B180" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C180" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D180" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E180" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F180" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G180" s="0" t="s">
+        <v>1420</v>
+      </c>
+      <c r="H180" s="0" t="s">
+        <v>608</v>
+      </c>
+      <c r="I180" s="0" t="s">
+        <v>1421</v>
+      </c>
+      <c r="J180" s="0" t="s">
+        <v>1422</v>
+      </c>
+      <c r="K180" s="0" t="s">
+        <v>1423</v>
+      </c>
+      <c r="L180" s="0" t="s">
+        <v>1424</v>
+      </c>
+      <c r="M180" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="N180" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="O180" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="P180" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q180" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="R180" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="S180" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="T180" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="U180" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="V180" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="W180" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="X180" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y180" s="0" t="s">
+        <v>1425</v>
+      </c>
+      <c r="Z180" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA180" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB180" s="0" t="s">
+        <v>1426</v>
+      </c>
+      <c r="AC180" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD180" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE180" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="AF180" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG180" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH180" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="AI180" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ180" s="0" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="181" spans="1:36">
+      <c r="A181" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B181" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C181" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D181" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E181" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F181" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G181" s="0" t="s">
+        <v>1427</v>
+      </c>
+      <c r="H181" s="0" t="s">
+        <v>1428</v>
+      </c>
+      <c r="I181" s="0" t="s">
+        <v>1429</v>
+      </c>
+      <c r="J181" s="0" t="s">
+        <v>1430</v>
+      </c>
+      <c r="K181" s="0" t="s">
+        <v>1431</v>
+      </c>
+      <c r="L181" s="0" t="s">
+        <v>1432</v>
+      </c>
+      <c r="M181" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="N181" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="O181" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="P181" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q181" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="R181" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="S181" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="T181" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="U181" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="V181" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="W181" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="X181" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y181" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z181" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA181" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB181" s="0" t="s">
+        <v>1433</v>
+      </c>
+      <c r="AC181" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD181" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE181" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="AF181" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG181" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH181" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="AI181" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ181" s="0" t="s">
+        <v>1434</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feature-candidate-login with registration linting
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>NILL</t>
   </si>
@@ -47,6 +47,30 @@
   </si>
   <si>
     <t>$2b$12$ESEMmLu3Wn30WG.Na1RHzO1Jr6k14tzSWikij9aUy7kljQqxhu5S2</t>
+  </si>
+  <si>
+    <t>xyz3</t>
+  </si>
+  <si>
+    <t>xyz3@bloombit.co</t>
+  </si>
+  <si>
+    <t>$2b$12$ESEMmLu3Wn30WG.Na1RHzOZbwNbZ6yFpF3a/4cCaHVN14.P5oQZk.</t>
+  </si>
+  <si>
+    <t>xyz4</t>
+  </si>
+  <si>
+    <t>xyz4@bloombit.co</t>
+  </si>
+  <si>
+    <t>xyz5</t>
+  </si>
+  <si>
+    <t>xyz5@bloombit.co</t>
+  </si>
+  <si>
+    <t>$2b$12$ESEMmLu3Wn30WG.Na1RHzOOqeVdluvxjmPMWLXNoOlnftwbykE/2O</t>
   </si>
 </sst>
 </file>
@@ -86,7 +110,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA4"/>
+  <dimension ref="A1:AA7"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -326,6 +350,252 @@
         <v>8</v>
       </c>
     </row>
+    <row r="5" spans="1:27">
+      <c r="A5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="R5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="S5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="T5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="U5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="V5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="W5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA5" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
+      <c r="A6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="O6" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="R6" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="S6" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="T6" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="U6" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="V6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W6" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="X6" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z6" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27">
+      <c r="A7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M7" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="N7" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="O7" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="P7" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="R7" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="S7" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="T7" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="U7" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="V7" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="W7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X7" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA7" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
mentor login and dashboard data display
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>NILL</t>
   </si>
@@ -203,6 +203,42 @@
   </si>
   <si>
     <t>9999999998</t>
+  </si>
+  <si>
+    <t>vd</t>
+  </si>
+  <si>
+    <t>dddddvdavd</t>
+  </si>
+  <si>
+    <t>vsdvvd@fbv.comdavdav</t>
+  </si>
+  <si>
+    <t>9988998897</t>
+  </si>
+  <si>
+    <t>33333</t>
+  </si>
+  <si>
+    <t>Rekonnect</t>
+  </si>
+  <si>
+    <t>Staging</t>
+  </si>
+  <si>
+    <t>rekonnectstaging@gmail.com</t>
+  </si>
+  <si>
+    <t>svd</t>
+  </si>
+  <si>
+    <t>asdv</t>
+  </si>
+  <si>
+    <t>sarvpalav@sarvedsh.comdavda</t>
+  </si>
+  <si>
+    <t>555555555</t>
   </si>
 </sst>
 </file>
@@ -242,7 +278,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB19"/>
+  <dimension ref="A1:AB22"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -1724,6 +1760,258 @@
         <v>34</v>
       </c>
     </row>
+    <row r="20" spans="1:28">
+      <c r="A20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="I20" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="J20" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="K20" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="L20" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M20" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="N20" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="O20" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="P20" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="R20" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="S20" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="T20" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="U20" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="V20" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="W20" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="X20" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z20" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26">
+      <c r="A21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="K21" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="L21" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M21" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="N21" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="O21" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="P21" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="R21" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="S21" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="T21" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="U21" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="V21" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="W21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X21" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28">
+      <c r="A22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="K22" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="L22" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M22" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="N22" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="O22" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="P22" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="R22" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="S22" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="T22" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="U22" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="V22" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="W22" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="X22" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z22" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
edit and add candidate dashboard
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -43,7 +43,7 @@
     <t>9998884488</t>
   </si>
   <si>
-    <t>553321</t>
+    <t>5555</t>
   </si>
   <si>
     <t/>
@@ -104,13 +104,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD3"/>
+  <dimension ref="A1:AC3"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:29">
       <c r="A2" s="0" t="s">
         <v>0</v>
       </c>
@@ -190,19 +190,16 @@
         <v>2</v>
       </c>
       <c r="AA2" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB2" s="0" t="s">
         <v>2</v>
       </c>
       <c r="AC2" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD2" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:29">
       <c r="A3" s="0" t="s">
         <v>0</v>
       </c>
@@ -282,15 +279,12 @@
         <v>2</v>
       </c>
       <c r="AA3" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB3" s="0" t="s">
         <v>2</v>
       </c>
       <c r="AC3" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD3" s="0" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>